<commit_message>
Added VRPTWUnviable and other stuff
</commit_message>
<xml_diff>
--- a/VRPTW-New/Zeus OS VRPTW Workspace 2018 2.4/Zeus/data/VRPTW/Results/S_ResultsSummary.xlsx
+++ b/VRPTW-New/Zeus OS VRPTW Workspace 2018 2.4/Zeus/data/VRPTW/Results/S_ResultsSummary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="32">
   <si>
     <t/>
   </si>
@@ -26,7 +26,28 @@
     <t>Insertion Type</t>
   </si>
   <si>
-    <t>CPU Time</t>
+    <t>CPU Time - Create Initial Routes</t>
+  </si>
+  <si>
+    <t>CPU Time - Total</t>
+  </si>
+  <si>
+    <t>Total Demand</t>
+  </si>
+  <si>
+    <t>Total Distance</t>
+  </si>
+  <si>
+    <t>Total Service Time</t>
+  </si>
+  <si>
+    <t>Total Waiting Time</t>
+  </si>
+  <si>
+    <t>Max Travel Time</t>
+  </si>
+  <si>
+    <t>Number of Trucks</t>
   </si>
   <si>
     <t>c101.xlsx</t>
@@ -150,887 +171,2231 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2164.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4631.328125</v>
+      </c>
+      <c r="H2" t="n">
+        <v>24350.42885733452</v>
+      </c>
+      <c r="I2" t="n">
+        <v>37981.75699187126</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D3" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>887.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4600.1630859375</v>
+      </c>
+      <c r="H3" t="n">
+        <v>18307.200760405245</v>
+      </c>
+      <c r="I3" t="n">
+        <v>31907.36393789548</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
         <v>17.0</v>
       </c>
+      <c r="E4" t="n">
+        <v>757.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3890.388427734375</v>
+      </c>
+      <c r="H4" t="n">
+        <v>11973.381343993304</v>
+      </c>
+      <c r="I4" t="n">
+        <v>24863.769775542376</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>17.0</v>
+        <v>14.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>686.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3007.449462890625</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4477.912366101295</v>
+      </c>
+      <c r="I5" t="n">
+        <v>16485.36183280662</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>726.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4582.802734375</v>
+      </c>
+      <c r="H6" t="n">
+        <v>24902.73081342841</v>
+      </c>
+      <c r="I6" t="n">
+        <v>38485.533332273015</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" t="n">
         <v>14.0</v>
       </c>
+      <c r="E7" t="n">
+        <v>640.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4444.40234375</v>
+      </c>
+      <c r="H7" t="n">
+        <v>20491.78412118256</v>
+      </c>
+      <c r="I7" t="n">
+        <v>33936.186623242495</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>45.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>651.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4481.662109375</v>
+      </c>
+      <c r="H8" t="n">
+        <v>20824.4270091596</v>
+      </c>
+      <c r="I8" t="n">
+        <v>34306.088994556936</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
       <c r="D9" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>728.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4246.5810546875</v>
+      </c>
+      <c r="H9" t="n">
+        <v>17995.245692372417</v>
+      </c>
+      <c r="I9" t="n">
+        <v>31241.826651692485</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>40.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>10.0</v>
+        <v>15.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3857.16845703125</v>
+      </c>
+      <c r="H10" t="n">
+        <v>11211.182270575979</v>
+      </c>
+      <c r="I10" t="n">
+        <v>24068.35065131328</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>31.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D11" t="n">
-        <v>26.0</v>
+        <v>33.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>777.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5770.96240234375</v>
+      </c>
+      <c r="H11" t="n">
+        <v>39798.69521595084</v>
+      </c>
+      <c r="I11" t="n">
+        <v>54569.65757061087</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>100.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D12" t="n">
         <v>25.0</v>
       </c>
+      <c r="E12" t="n">
+        <v>669.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4954.9609375</v>
+      </c>
+      <c r="H12" t="n">
+        <v>27102.645037524635</v>
+      </c>
+      <c r="I12" t="n">
+        <v>41057.6061619448</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>77.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
         <v>19.0</v>
       </c>
+      <c r="E13" t="n">
+        <v>625.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3904.415283203125</v>
+      </c>
+      <c r="H13" t="n">
+        <v>19512.288545377014</v>
+      </c>
+      <c r="I13" t="n">
+        <v>32416.70374274945</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D14" t="n">
-        <v>10.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>589.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2967.667236328125</v>
+      </c>
+      <c r="H14" t="n">
+        <v>9250.297419156943</v>
+      </c>
+      <c r="I14" t="n">
+        <v>21217.96476801864</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>32.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D15" t="n">
-        <v>21.0</v>
+        <v>27.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>660.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5322.0888671875</v>
+      </c>
+      <c r="H15" t="n">
+        <v>36312.579631916335</v>
+      </c>
+      <c r="I15" t="n">
+        <v>50634.66844951277</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>88.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D16" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5215.412109375</v>
+      </c>
+      <c r="H16" t="n">
+        <v>34120.520738819585</v>
+      </c>
+      <c r="I16" t="n">
+        <v>48335.93297789429</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>85.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D17" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>632.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5324.14208984375</v>
+      </c>
+      <c r="H17" t="n">
+        <v>33501.38956122964</v>
+      </c>
+      <c r="I17" t="n">
+        <v>47825.53183036416</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>83.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D18" t="n">
-        <v>18.0</v>
+        <v>16.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>607.0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4995.25146484375</v>
+      </c>
+      <c r="H18" t="n">
+        <v>29257.279647460266</v>
+      </c>
+      <c r="I18" t="n">
+        <v>43252.53126298456</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>72.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D19" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>693.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>4521.708984375</v>
+      </c>
+      <c r="H19" t="n">
+        <v>23757.54489263449</v>
+      </c>
+      <c r="I19" t="n">
+        <v>37279.254065837005</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>61.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D20" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>509.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3120.250732421875</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5042.796046458685</v>
+      </c>
+      <c r="I20" t="n">
+        <v>17163.04687806269</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>21.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D21" t="n">
         <v>4.0</v>
       </c>
+      <c r="E21" t="n">
+        <v>487.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3145.373291015625</v>
+      </c>
+      <c r="H21" t="n">
+        <v>3585.2597240832483</v>
+      </c>
+      <c r="I21" t="n">
+        <v>15730.63304561645</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D22" t="n">
         <v>4.0</v>
       </c>
+      <c r="E22" t="n">
+        <v>512.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2708.929443359375</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3511.0554530863355</v>
+      </c>
+      <c r="I22" t="n">
+        <v>15219.984791541536</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D23" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>495.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2008.2159423828125</v>
+      </c>
+      <c r="H23" t="n">
+        <v>3024.4800800166795</v>
+      </c>
+      <c r="I23" t="n">
+        <v>14032.696022399492</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>16.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D24" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3228.932861328125</v>
+      </c>
+      <c r="H24" t="n">
+        <v>3383.8572770694655</v>
+      </c>
+      <c r="I24" t="n">
+        <v>15612.790191803353</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>18.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D25" t="n">
         <v>3.0</v>
       </c>
+      <c r="E25" t="n">
+        <v>504.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3282.5771484375</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3520.6178415658715</v>
+      </c>
+      <c r="I25" t="n">
+        <v>15803.195043409134</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>18.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D26" t="n">
         <v>3.0</v>
       </c>
+      <c r="E26" t="n">
+        <v>511.0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3132.698974609375</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3056.6980366649736</v>
+      </c>
+      <c r="I26" t="n">
+        <v>15189.397011274348</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D27" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>487.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2930.08056640625</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1488.8676282278368</v>
+      </c>
+      <c r="I27" t="n">
+        <v>13418.94824803985</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>14.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D28" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>477.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2971.502197265625</v>
+      </c>
+      <c r="H28" t="n">
+        <v>808.6965173444326</v>
+      </c>
+      <c r="I28" t="n">
+        <v>12780.19860016914</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>12.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D29" t="n">
-        <v>106.0</v>
+        <v>107.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>745.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4385.32763671875</v>
+      </c>
+      <c r="H29" t="n">
+        <v>19448.456801232212</v>
+      </c>
+      <c r="I29" t="n">
+        <v>32833.78448372733</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D30" t="n">
-        <v>134.0</v>
+        <v>150.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>871.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4049.98388671875</v>
+      </c>
+      <c r="H30" t="n">
+        <v>13722.286826858985</v>
+      </c>
+      <c r="I30" t="n">
+        <v>26772.27069068955</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D31" t="n">
-        <v>143.0</v>
+        <v>106.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>776.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4297.9951171875</v>
+      </c>
+      <c r="H31" t="n">
+        <v>9538.398278110984</v>
+      </c>
+      <c r="I31" t="n">
+        <v>22836.393242710594</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D32" t="n">
-        <v>40.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>704.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4975.4951171875</v>
+      </c>
+      <c r="H32" t="n">
+        <v>4829.577076615016</v>
+      </c>
+      <c r="I32" t="n">
+        <v>18805.07202214114</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>67.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D33" t="n">
-        <v>121.0</v>
+        <v>75.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>700.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4481.77880859375</v>
+      </c>
+      <c r="H33" t="n">
+        <v>20423.413446118466</v>
+      </c>
+      <c r="I33" t="n">
+        <v>33905.192411114804</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D34" t="n">
-        <v>49.0</v>
+        <v>50.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>656.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>4296.0849609375</v>
+      </c>
+      <c r="H34" t="n">
+        <v>14325.074087506011</v>
+      </c>
+      <c r="I34" t="n">
+        <v>27621.159143810943</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>41.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D35" t="n">
-        <v>126.0</v>
+        <v>130.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>730.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4326.03173828125</v>
+      </c>
+      <c r="H35" t="n">
+        <v>16606.57567153384</v>
+      </c>
+      <c r="I35" t="n">
+        <v>29932.6073945563</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>48.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D36" t="n">
-        <v>35.0</v>
+        <v>30.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>800.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3889.284423828125</v>
+      </c>
+      <c r="H36" t="n">
+        <v>10507.48369979126</v>
+      </c>
+      <c r="I36" t="n">
+        <v>23396.76817321045</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>37.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D37" t="n">
-        <v>132.0</v>
+        <v>137.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>670.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3735.349365234375</v>
+      </c>
+      <c r="H37" t="n">
+        <v>5515.188610131957</v>
+      </c>
+      <c r="I37" t="n">
+        <v>18250.537876184204</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>32.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D38" t="n">
-        <v>39.0</v>
+        <v>43.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>627.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>4316.5615234375</v>
+      </c>
+      <c r="H38" t="n">
+        <v>26082.198277881685</v>
+      </c>
+      <c r="I38" t="n">
+        <v>39398.759793689795</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>64.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D39" t="n">
-        <v>46.0</v>
+        <v>44.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>794.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3783.201416015625</v>
+      </c>
+      <c r="H39" t="n">
+        <v>16617.39224616174</v>
+      </c>
+      <c r="I39" t="n">
+        <v>29400.593665992063</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>52.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D40" t="n">
-        <v>49.0</v>
+        <v>56.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>762.0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3000.89013671875</v>
+      </c>
+      <c r="H40" t="n">
+        <v>10829.521665972796</v>
+      </c>
+      <c r="I40" t="n">
+        <v>22830.41175310048</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>39.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D41" t="n">
-        <v>29.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>683.0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2772.92724609375</v>
+      </c>
+      <c r="H41" t="n">
+        <v>6046.483656547029</v>
+      </c>
+      <c r="I41" t="n">
+        <v>17819.41091599222</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>35.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D42" t="n">
-        <v>22.0</v>
+        <v>28.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>752.0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3988.114990234375</v>
+      </c>
+      <c r="H42" t="n">
+        <v>17816.50821463221</v>
+      </c>
+      <c r="I42" t="n">
+        <v>30804.623258272346</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>54.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D43" t="n">
-        <v>32.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>690.0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3911.18359375</v>
+      </c>
+      <c r="H43" t="n">
+        <v>19057.812691301915</v>
+      </c>
+      <c r="I43" t="n">
+        <v>31968.996243090245</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>57.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D44" t="n">
-        <v>31.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>787.0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>4158.77685546875</v>
+      </c>
+      <c r="H44" t="n">
+        <v>17624.16312242266</v>
+      </c>
+      <c r="I44" t="n">
+        <v>30782.93993592974</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>58.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D45" t="n">
-        <v>32.0</v>
+        <v>46.0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>757.0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3362.16259765625</v>
+      </c>
+      <c r="H45" t="n">
+        <v>13276.557793662872</v>
+      </c>
+      <c r="I45" t="n">
+        <v>25638.720425651398</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>46.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D46" t="n">
-        <v>30.0</v>
+        <v>32.0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>697.0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3045.95703125</v>
+      </c>
+      <c r="H46" t="n">
+        <v>7166.263516447239</v>
+      </c>
+      <c r="I46" t="n">
+        <v>19212.22047521799</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>38.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D47" t="n">
-        <v>19.0</v>
+        <v>27.0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>673.0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>4535.7314453125</v>
+      </c>
+      <c r="H47" t="n">
+        <v>24292.129521046252</v>
+      </c>
+      <c r="I47" t="n">
+        <v>37827.86109605846</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>68.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D48" t="n">
-        <v>23.0</v>
+        <v>22.0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>691.0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3610.64404296875</v>
+      </c>
+      <c r="H48" t="n">
+        <v>13910.755266599946</v>
+      </c>
+      <c r="I48" t="n">
+        <v>26521.399420194917</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>51.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D49" t="n">
-        <v>40.0</v>
+        <v>68.0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>713.0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>3688.30224609375</v>
+      </c>
+      <c r="H49" t="n">
+        <v>9098.722617665751</v>
+      </c>
+      <c r="I49" t="n">
+        <v>21787.024804631692</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>53.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D50" t="n">
-        <v>57.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>639.0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5032.4541015625</v>
+      </c>
+      <c r="H50" t="n">
+        <v>4504.430079758286</v>
+      </c>
+      <c r="I50" t="n">
+        <v>18536.88441401732</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>77.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D51" t="n">
         <v>5.0</v>
       </c>
+      <c r="E51" t="n">
+        <v>629.0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4693.80419921875</v>
+      </c>
+      <c r="H51" t="n">
+        <v>19246.269539453806</v>
+      </c>
+      <c r="I51" t="n">
+        <v>32940.07382641059</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>64.0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D52" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>705.0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>4614.46044921875</v>
+      </c>
+      <c r="H52" t="n">
+        <v>22381.953958522343</v>
+      </c>
+      <c r="I52" t="n">
+        <v>35996.41429711487</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>67.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D53" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>641.0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>4403.265625</v>
+      </c>
+      <c r="H53" t="n">
+        <v>19279.695014086356</v>
+      </c>
+      <c r="I53" t="n">
+        <v>32682.960650530447</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>60.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D54" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>632.0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3666.9677734375</v>
+      </c>
+      <c r="H54" t="n">
+        <v>14272.897365567474</v>
+      </c>
+      <c r="I54" t="n">
+        <v>26939.86508941391</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D55" t="n">
-        <v>10.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>525.0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>2566.471923828125</v>
+      </c>
+      <c r="H55" t="n">
+        <v>7249.700764184713</v>
+      </c>
+      <c r="I55" t="n">
+        <v>18816.172722345113</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D56" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>572.0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2682.7685546875</v>
+      </c>
+      <c r="H56" t="n">
+        <v>4392.980240782195</v>
+      </c>
+      <c r="I56" t="n">
+        <v>16075.748856504852</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>19.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D57" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>514.0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>2531.57080078125</v>
+      </c>
+      <c r="H57" t="n">
+        <v>4713.8407006869265</v>
+      </c>
+      <c r="I57" t="n">
+        <v>16245.411493838783</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>18.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D58" t="n">
         <v>3.0</v>
       </c>
+      <c r="E58" t="n">
+        <v>519.0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>2290.24658203125</v>
+      </c>
+      <c r="H58" t="n">
+        <v>6408.222738893873</v>
+      </c>
+      <c r="I58" t="n">
+        <v>17698.46943536604</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D59" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1697.856201171875</v>
+      </c>
+      <c r="H59" t="n">
+        <v>5199.678139453631</v>
+      </c>
+      <c r="I59" t="n">
+        <v>15897.534371143083</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>15.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D60" t="n">
         <v>3.0</v>
       </c>
+      <c r="E60" t="n">
+        <v>515.0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>2732.649658203125</v>
+      </c>
+      <c r="H60" t="n">
+        <v>2852.222217150221</v>
+      </c>
+      <c r="I60" t="n">
+        <v>14584.871783800612</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D61" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>488.0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>2594.1005859375</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3499.0598682415416</v>
+      </c>
+      <c r="I61" t="n">
+        <v>15093.160377885097</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>17.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D62" t="n">
         <v>3.0</v>
       </c>
+      <c r="E62" t="n">
+        <v>484.0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>2649.6181640625</v>
+      </c>
+      <c r="H62" t="n">
+        <v>2204.738854535072</v>
+      </c>
+      <c r="I62" t="n">
+        <v>13854.356980450599</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D63" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>463.0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>2150.9677734375</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1490.7987450557005</v>
+      </c>
+      <c r="I63" t="n">
+        <v>12641.766411681678</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K63" t="n">
+        <v>14.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D64" t="n">
         <v>3.0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>463.0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1810.0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1949.1329345703125</v>
+      </c>
+      <c r="H64" t="n">
+        <v>1185.8000635806072</v>
+      </c>
+      <c r="I64" t="n">
+        <v>12134.932952374553</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>13.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>